<commit_message>
added try catch in all test cases and completed theme scripts
</commit_message>
<xml_diff>
--- a/src/test/java/rc25/mFormsAutomation/TestData/Theme.xlsx
+++ b/src/test/java/rc25/mFormsAutomation/TestData/Theme.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="5" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Edit Theme" sheetId="2" r:id="rId3"/>
     <sheet name="View Theme" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -375,16 +375,16 @@
     <t>Valid theme name which you want to view</t>
   </si>
   <si>
-    <t>Super admin theme</t>
-  </si>
-  <si>
     <t>Theme 2888</t>
   </si>
   <si>
-    <t>Theme 154354</t>
-  </si>
-  <si>
     <t>Astegic1!</t>
+  </si>
+  <si>
+    <t>seltest12</t>
+  </si>
+  <si>
+    <t>SelTest14</t>
   </si>
 </sst>
 </file>
@@ -794,7 +794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -820,7 +820,7 @@
         <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
         <v>30</v>
@@ -835,7 +835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -941,7 +941,7 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>11</v>

</xml_diff>